<commit_message>
Update barley trait ontology and sprout tolerance trait
</commit_message>
<xml_diff>
--- a/ontology/hordeum-props.xlsx
+++ b/ontology/hordeum-props.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="361">
   <si>
     <t>trait_name</t>
   </si>
@@ -1091,6 +1091,12 @@
   </si>
   <si>
     <t>TRAIT: Fusarium Head Blight incidence ::: METHOD: Fusarium Head Blight incidence - 20 HC - Computation ::: SCALE: %</t>
+  </si>
+  <si>
+    <t>Sprouting tolerance - 1-9 TOL scale</t>
+  </si>
+  <si>
+    <t>TRAIT: Sprouting tolerance ::: METHOD: SproutTol Estimation ::: SCALE: 1-9 TOL scale</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H166"/>
+  <dimension ref="A1:H167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3398,6 +3404,17 @@
         <v>358</v>
       </c>
     </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>359</v>
+      </c>
+      <c r="F167" t="s">
+        <v>37</v>
+      </c>
+      <c r="G167" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>